<commit_message>
Add suggest for import
</commit_message>
<xml_diff>
--- a/sparepart.xlsx
+++ b/sparepart.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Id</t>
   </si>
@@ -23,36 +23,6 @@
   </si>
   <si>
     <t>Qty</t>
-  </si>
-  <si>
-    <t>Dao phay ngón phi 3</t>
-  </si>
-  <si>
-    <t>3S4</t>
-  </si>
-  <si>
-    <t>kim khâu 121</t>
-  </si>
-  <si>
-    <t>kh001</t>
-  </si>
-  <si>
-    <t>Mũi khoan  phi 5</t>
-  </si>
-  <si>
-    <t>5mm</t>
-  </si>
-  <si>
-    <t>khuy áo 1111</t>
-  </si>
-  <si>
-    <t>ka001</t>
-  </si>
-  <si>
-    <t>vật tư 1</t>
-  </si>
-  <si>
-    <t>p1234</t>
   </si>
 </sst>
 </file>
@@ -429,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
@@ -450,160 +420,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>4</v>
-      </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>3</v>
-      </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>2</v>
-      </c>
-      <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>